<commit_message>
Append new water filling record
</commit_message>
<xml_diff>
--- a/Database/Data.xlsx
+++ b/Database/Data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="سجل" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -428,9 +428,35 @@
         <v>ملاحظات</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>a</v>
+      </c>
+      <c r="B2" t="str">
+        <v>b</v>
+      </c>
+      <c r="C2" t="str">
+        <v>c</v>
+      </c>
+      <c r="D2" t="str">
+        <v>d</v>
+      </c>
+      <c r="E2" t="str">
+        <v>w</v>
+      </c>
+      <c r="F2" t="str">
+        <v>e</v>
+      </c>
+      <c r="G2" t="str">
+        <v>f</v>
+      </c>
+      <c r="H2" t="str">
+        <v>g</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append new row via script
</commit_message>
<xml_diff>
--- a/Database/Data.xlsx
+++ b/Database/Data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -480,9 +480,35 @@
         <v>az</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>12</v>
+      </c>
+      <c r="B4" t="str">
+        <v>34</v>
+      </c>
+      <c r="C4" t="str">
+        <v>12</v>
+      </c>
+      <c r="D4" t="str">
+        <v>6</v>
+      </c>
+      <c r="E4" t="str">
+        <v>6</v>
+      </c>
+      <c r="F4" t="str">
+        <v>7</v>
+      </c>
+      <c r="G4" t="str">
+        <v>8</v>
+      </c>
+      <c r="H4" t="str">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append row at 2025-05-01T11:00:11.932Z
</commit_message>
<xml_diff>
--- a/Database/Data.xlsx
+++ b/Database/Data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -506,9 +506,35 @@
         <v>9</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>2025-05-01T11:00:11.932Z</v>
+      </c>
+      <c r="B5" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="C5" t="str">
+        <v>C3</v>
+      </c>
+      <c r="D5" t="str">
+        <v>أخرى</v>
+      </c>
+      <c r="E5" t="str">
+        <v>الصمود</v>
+      </c>
+      <c r="F5" t="str">
+        <v>احمد</v>
+      </c>
+      <c r="G5" t="str">
+        <v>32</v>
+      </c>
+      <c r="H5" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append row at 01‏/05‏/2025 02:07:49 م
</commit_message>
<xml_diff>
--- a/Database/Data.xlsx
+++ b/Database/Data.xlsx
@@ -1,55 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hasan Saleh\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
-  </bookViews>
   <sheets>
     <sheet name="سجل" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>المؤسسة</t>
-  </si>
-  <si>
-    <t>المركبة</t>
-  </si>
-  <si>
-    <t>المخيم</t>
-  </si>
-  <si>
-    <t>الكمية</t>
-  </si>
-  <si>
-    <t>المرافق</t>
-  </si>
-  <si>
-    <t>ملاحظات</t>
-  </si>
-  <si>
-    <t>نوع المسافة</t>
-  </si>
-  <si>
-    <t>الوقت</t>
-  </si>
-</sst>
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -78,25 +64,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -421,52 +396,67 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="25.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="22.125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.25" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.75" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9" style="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>ملاحظات</v>
+      </c>
+      <c r="B1" t="str">
+        <v>المرافق</v>
+      </c>
+      <c r="C1" t="str">
+        <v>الكمية</v>
+      </c>
+      <c r="D1" t="str">
+        <v>المخيم</v>
+      </c>
+      <c r="E1" t="str">
+        <v>نوع المسافة</v>
+      </c>
+      <c r="F1" t="str">
+        <v>المركبة</v>
+      </c>
+      <c r="G1" t="str">
+        <v>المؤسسة</v>
+      </c>
+      <c r="H1" t="str">
+        <v>الوقت</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>01‏/05‏/2025 02:07:49 م</v>
+      </c>
+      <c r="B2" t="str">
+        <v>IDRF</v>
+      </c>
+      <c r="C2" t="str">
+        <v>C2</v>
+      </c>
+      <c r="D2" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="E2" t="str">
+        <v>الصمود</v>
+      </c>
+      <c r="F2" t="str">
+        <v>أحمد شريم</v>
+      </c>
+      <c r="G2" t="str">
+        <v>1212</v>
+      </c>
+      <c r="H2" t="str">
+        <v/>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append row at 01‏/05‏/2025 02:08:51 م
</commit_message>
<xml_diff>
--- a/Database/Data.xlsx
+++ b/Database/Data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -454,9 +454,35 @@
         <v/>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>01‏/05‏/2025 02:08:51 م</v>
+      </c>
+      <c r="B3" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="C3" t="str">
+        <v>C4</v>
+      </c>
+      <c r="D3" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="E3" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="F3" t="str">
+        <v>احمد</v>
+      </c>
+      <c r="G3" t="str">
+        <v>222</v>
+      </c>
+      <c r="H3" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append row at 01‏/05‏/2025 02:11:35 م
</commit_message>
<xml_diff>
--- a/Database/Data.xlsx
+++ b/Database/Data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -480,9 +480,35 @@
         <v/>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>01‏/05‏/2025 02:11:35 م</v>
+      </c>
+      <c r="B4" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="C4" t="str">
+        <v>C2</v>
+      </c>
+      <c r="D4" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="E4" t="str">
+        <v>بير 19</v>
+      </c>
+      <c r="F4" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="G4" t="str">
+        <v>2323</v>
+      </c>
+      <c r="H4" t="str">
+        <v>واو</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append row at 01‏/05‏/2025 02:12:45 م
</commit_message>
<xml_diff>
--- a/Database/Data.xlsx
+++ b/Database/Data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -506,9 +506,35 @@
         <v>واو</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>01‏/05‏/2025 02:12:45 م</v>
+      </c>
+      <c r="B5" t="str">
+        <v>WCK</v>
+      </c>
+      <c r="C5" t="str">
+        <v>C3</v>
+      </c>
+      <c r="D5" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="E5" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="F5" t="str">
+        <v>احمد</v>
+      </c>
+      <c r="G5" t="str">
+        <v>23223</v>
+      </c>
+      <c r="H5" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append row at 2025-05-01T11:14:47.873Z
</commit_message>
<xml_diff>
--- a/Database/Data.xlsx
+++ b/Database/Data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -532,9 +532,35 @@
         <v/>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>2025-05-01T11:14:47.873Z</v>
+      </c>
+      <c r="B6" t="str">
+        <v>IDRF</v>
+      </c>
+      <c r="C6" t="str">
+        <v>C3</v>
+      </c>
+      <c r="D6" t="str">
+        <v>الرحلة 1</v>
+      </c>
+      <c r="E6" t="str">
+        <v>الصمود</v>
+      </c>
+      <c r="F6" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="G6" t="str">
+        <v>12</v>
+      </c>
+      <c r="H6" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append row at 2025-05-01T11:17:19.059Z
</commit_message>
<xml_diff>
--- a/Database/Data.xlsx
+++ b/Database/Data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -558,9 +558,35 @@
         <v/>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>2025-05-01T11:17:19.059Z</v>
+      </c>
+      <c r="B7" t="str">
+        <v>IDRF</v>
+      </c>
+      <c r="C7" t="str">
+        <v>C3</v>
+      </c>
+      <c r="D7" t="str">
+        <v>الرحلة 1</v>
+      </c>
+      <c r="E7" t="str">
+        <v>الصمود</v>
+      </c>
+      <c r="F7" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="G7" t="str">
+        <v>123123</v>
+      </c>
+      <c r="H7" t="str">
+        <v>123</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append row at 2025-05-01T11:18:34.545Z
</commit_message>
<xml_diff>
--- a/Database/Data.xlsx
+++ b/Database/Data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -584,9 +584,35 @@
         <v>123</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>2025-05-01T11:18:34.545Z</v>
+      </c>
+      <c r="B8" t="str">
+        <v>IDRF</v>
+      </c>
+      <c r="C8" t="str">
+        <v>C3</v>
+      </c>
+      <c r="D8" t="str">
+        <v>الرحلة 1</v>
+      </c>
+      <c r="E8" t="str">
+        <v>الصمود</v>
+      </c>
+      <c r="F8" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="G8" t="str">
+        <v>123123</v>
+      </c>
+      <c r="H8" t="str">
+        <v>123</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append row at 2025-05-01T11:47:45.706Z
</commit_message>
<xml_diff>
--- a/Database/Data.xlsx
+++ b/Database/Data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -792,9 +792,35 @@
         <v/>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>2025-05-01T11:47:45.694Z</v>
+      </c>
+      <c r="B16" t="str">
+        <v>UNDP</v>
+      </c>
+      <c r="C16" t="str">
+        <v>C4</v>
+      </c>
+      <c r="D16" t="str">
+        <v>الرحلة 3</v>
+      </c>
+      <c r="E16" t="str">
+        <v>الصمود</v>
+      </c>
+      <c r="F16" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="G16" t="str">
+        <v>421123</v>
+      </c>
+      <c r="H16" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H15"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H16"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append row at 2025-05-01T11:48:55.200Z
</commit_message>
<xml_diff>
--- a/Database/Data.xlsx
+++ b/Database/Data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -818,9 +818,35 @@
         <v/>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>2025-05-01T11:48:55.200Z</v>
+      </c>
+      <c r="B17" t="str">
+        <v>UNDP</v>
+      </c>
+      <c r="C17" t="str">
+        <v>C4</v>
+      </c>
+      <c r="D17" t="str">
+        <v>الرحلة 3</v>
+      </c>
+      <c r="E17" t="str">
+        <v>الصمود</v>
+      </c>
+      <c r="F17" t="str">
+        <v xml:space="preserve">يامن </v>
+      </c>
+      <c r="G17" t="str">
+        <v>43434</v>
+      </c>
+      <c r="H17" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H16"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H17"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append row at 2025-05-01T11:50:26.484Z
</commit_message>
<xml_diff>
--- a/Database/Data.xlsx
+++ b/Database/Data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -844,9 +844,35 @@
         <v/>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>2025-05-01T11:50:26.484Z</v>
+      </c>
+      <c r="B18" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="C18" t="str">
+        <v>C3</v>
+      </c>
+      <c r="D18" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="E18" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="F18" t="str">
+        <v>احمد</v>
+      </c>
+      <c r="G18" t="str">
+        <v>2323</v>
+      </c>
+      <c r="H18" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H17"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H18"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append row at 2025-05-01T11:53:37.511Z
</commit_message>
<xml_diff>
--- a/Database/Data.xlsx
+++ b/Database/Data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -870,9 +870,35 @@
         <v/>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>2025-05-01T11:53:37.511Z</v>
+      </c>
+      <c r="B19" t="str">
+        <v>UNICEF</v>
+      </c>
+      <c r="C19" t="str">
+        <v>C3</v>
+      </c>
+      <c r="D19" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="E19" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="F19" t="str">
+        <v>احمد</v>
+      </c>
+      <c r="G19" t="str">
+        <v>1212</v>
+      </c>
+      <c r="H19" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H18"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H19"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>